<commit_message>
built: requirements and add text
</commit_message>
<xml_diff>
--- a/Requirement Model Loader.xlsx
+++ b/Requirement Model Loader.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivia\Git\Bird_Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A80A0-DDAA-4BEA-AA86-D98E67962E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7327FE6-E1B2-4DC3-B050-E6CFC5599EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02421E9F-6F91-4F88-92F9-C987603F6219}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Use Case ID:</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>Use Case Name:</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Return prediction</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,67 +644,67 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="2:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="2:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -717,7 +717,7 @@
     </row>
     <row r="10" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -725,16 +725,16 @@
     </row>
     <row r="11" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -742,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -756,13 +756,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -770,13 +770,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -784,13 +784,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -798,13 +798,13 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -812,13 +812,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -826,13 +826,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -840,13 +840,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -854,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -868,13 +868,13 @@
         <v>10</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>